<commit_message>
Add commands for resetting git credentials
</commit_message>
<xml_diff>
--- a/src/spreadsheets/git.xlsx
+++ b/src/spreadsheets/git.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\developers-cheat-sheet\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\developers-cheat-sheet\src\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8C803F-A599-4632-8F47-6349276050D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FEEE32-8451-4E72-8D73-08C776B7D640}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{AC50BE90-470E-4ADB-ABB4-54CE8C3071A4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Action</t>
   </si>
@@ -62,14 +62,6 @@
     <t>Stash uncommitted changes</t>
   </si>
   <si>
-    <t>git stash
-git stash push -m "&lt;stash-name&gt;"
-(switch branches)
-git stash apply
-git stash list
-git stash apply stash@{1}</t>
-  </si>
-  <si>
     <t>Undo a commit</t>
   </si>
   <si>
@@ -78,11 +70,6 @@
   </si>
   <si>
     <t>Add a remote</t>
-  </si>
-  <si>
-    <t>git remote add origin https://github.com/&lt;username&gt;/&lt;repo-name&gt;.git
-(make a commit)
-git push --set-upstream origin master</t>
   </si>
   <si>
     <t>Rename a branch (local+remote)</t>
@@ -99,6 +86,28 @@
   <si>
     <t>git push origin --delete &lt;remote-branch-name&gt;
 git branch -d &lt;local-branch-name&gt;</t>
+  </si>
+  <si>
+    <t>Reset git credentials</t>
+  </si>
+  <si>
+    <t>(For Mac)
+git config --global credential.helper osxkeychain
+(Credentials will be asked on next pull/push)
+(For Windows, reset from Windows Credentials Manager)</t>
+  </si>
+  <si>
+    <t>git remote add origin https://github.com/&lt;username&gt;/&lt;repo-name&gt;.git
+(Make a commit)
+git push --set-upstream origin master</t>
+  </si>
+  <si>
+    <t>git stash
+git stash push -m "&lt;stash-name&gt;"
+(Switch branches)
+git stash apply
+git stash list
+git stash apply stash@{1}</t>
   </si>
 </sst>
 </file>
@@ -462,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1EDD08-339E-4F53-A8CC-87B11A1193DB}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -503,38 +512,46 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>